<commit_message>
Cambios para el manejo de vistas de terminal y cambio de la variables de reseteo de hora al cambio de dia
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -17,13 +17,14 @@
     <sheet name="Hoja8" sheetId="8" r:id="rId8"/>
     <sheet name="Hoja9" sheetId="9" r:id="rId9"/>
     <sheet name="Hoja10" sheetId="10" r:id="rId10"/>
+    <sheet name="Hoja11" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="487">
   <si>
     <t>No</t>
   </si>
@@ -3845,6 +3846,2859 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F142"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>482</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0.116</v>
+      </c>
+      <c r="D2">
+        <v>0.066</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>483</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>0.078</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>484</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="D4">
+        <v>0.012</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>485</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>0.122</v>
+      </c>
+      <c r="D5">
+        <v>0.078</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>486</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>0.08</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>487</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>0.094</v>
+      </c>
+      <c r="D7">
+        <v>0.028</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>488</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+      <c r="D8">
+        <v>0.038</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>489</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>0.082</v>
+      </c>
+      <c r="D9">
+        <v>0.004</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>490</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>0.116</v>
+      </c>
+      <c r="D10">
+        <v>0.06</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>491</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>0.09</v>
+      </c>
+      <c r="D11">
+        <v>0.02</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>492</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>0.094</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>493</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>0.148</v>
+      </c>
+      <c r="D13">
+        <v>0.064</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>494</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>0.178</v>
+      </c>
+      <c r="D14">
+        <v>0.04</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>495</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>0.178</v>
+      </c>
+      <c r="D15">
+        <v>0.01</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>496</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>0.12</v>
+      </c>
+      <c r="D16">
+        <v>0.006</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>497</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>0.168</v>
+      </c>
+      <c r="D17">
+        <v>0.076</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>498</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>0.148</v>
+      </c>
+      <c r="D18">
+        <v>0.052</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>499</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>0.116</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>500</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>0.122</v>
+      </c>
+      <c r="D20">
+        <v>0.012</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>501</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>0.124</v>
+      </c>
+      <c r="D21">
+        <v>0.026</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>502</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22">
+        <v>0.138</v>
+      </c>
+      <c r="D22">
+        <v>0.068</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>503</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>504</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24">
+        <v>0.064</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>505</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25">
+        <v>0.134</v>
+      </c>
+      <c r="D25">
+        <v>0.004</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>506</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <v>0.264</v>
+      </c>
+      <c r="D26">
+        <v>0.068</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>507</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>0.15</v>
+      </c>
+      <c r="D27">
+        <v>0.036</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>508</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28">
+        <v>0.132</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>509</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <v>0.192</v>
+      </c>
+      <c r="D29">
+        <v>0.064</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>510</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30">
+        <v>0.172</v>
+      </c>
+      <c r="D30">
+        <v>0.014</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>511</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31">
+        <v>0.186</v>
+      </c>
+      <c r="D31">
+        <v>0.018</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>512</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32">
+        <v>0.184</v>
+      </c>
+      <c r="D32">
+        <v>0.056</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>513</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33">
+        <v>0.144</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>514</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34">
+        <v>0.142</v>
+      </c>
+      <c r="D34">
+        <v>0.042</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>515</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="D35">
+        <v>0.032</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>516</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36">
+        <v>0.1</v>
+      </c>
+      <c r="D36">
+        <v>0.01</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>517</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37">
+        <v>0.124</v>
+      </c>
+      <c r="D37">
+        <v>0.056</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>518</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="D38">
+        <v>0.01</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>519</v>
+      </c>
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="D39">
+        <v>0.002</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>520</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40">
+        <v>0.122</v>
+      </c>
+      <c r="D40">
+        <v>0.062</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>521</v>
+      </c>
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41">
+        <v>0.076</v>
+      </c>
+      <c r="D41">
+        <v>0.002</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>522</v>
+      </c>
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42">
+        <v>0.102</v>
+      </c>
+      <c r="D42">
+        <v>0.038</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>523</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43">
+        <v>0.096</v>
+      </c>
+      <c r="D43">
+        <v>0.044</v>
+      </c>
+      <c r="E43">
+        <v>0.002</v>
+      </c>
+      <c r="F43">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>524</v>
+      </c>
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>525</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45">
+        <v>0.096</v>
+      </c>
+      <c r="D45">
+        <v>0.044</v>
+      </c>
+      <c r="E45">
+        <v>0.002</v>
+      </c>
+      <c r="F45">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>526</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46">
+        <v>0.08</v>
+      </c>
+      <c r="D46">
+        <v>0.02</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>527</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47">
+        <v>0.08599999999999999</v>
+      </c>
+      <c r="D47">
+        <v>0.012</v>
+      </c>
+      <c r="E47">
+        <v>0.002</v>
+      </c>
+      <c r="F47">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>528</v>
+      </c>
+      <c r="B48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48">
+        <v>0.11</v>
+      </c>
+      <c r="D48">
+        <v>0.066</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>529</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49">
+        <v>0.06</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0.002</v>
+      </c>
+      <c r="F49">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>530</v>
+      </c>
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50">
+        <v>0.066</v>
+      </c>
+      <c r="D50">
+        <v>0.018</v>
+      </c>
+      <c r="E50">
+        <v>0.002</v>
+      </c>
+      <c r="F50">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>531</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51">
+        <v>0.098</v>
+      </c>
+      <c r="D51">
+        <v>0.048</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>532</v>
+      </c>
+      <c r="B52" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="D52">
+        <v>0.014</v>
+      </c>
+      <c r="E52">
+        <v>0.002</v>
+      </c>
+      <c r="F52">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>533</v>
+      </c>
+      <c r="B53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53">
+        <v>0.15</v>
+      </c>
+      <c r="D53">
+        <v>0.05</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>534</v>
+      </c>
+      <c r="B54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54">
+        <v>0.146</v>
+      </c>
+      <c r="D54">
+        <v>0.026</v>
+      </c>
+      <c r="E54">
+        <v>0.002</v>
+      </c>
+      <c r="F54">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>535</v>
+      </c>
+      <c r="B55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55">
+        <v>0.122</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>536</v>
+      </c>
+      <c r="B56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56">
+        <v>0.182</v>
+      </c>
+      <c r="D56">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E56">
+        <v>0.002</v>
+      </c>
+      <c r="F56">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>537</v>
+      </c>
+      <c r="B57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57">
+        <v>0.174</v>
+      </c>
+      <c r="D57">
+        <v>0.018</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <v>538</v>
+      </c>
+      <c r="B58" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58">
+        <v>0.158</v>
+      </c>
+      <c r="D58">
+        <v>0.028</v>
+      </c>
+      <c r="E58">
+        <v>0.002</v>
+      </c>
+      <c r="F58">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <v>539</v>
+      </c>
+      <c r="B59" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59">
+        <v>0.212</v>
+      </c>
+      <c r="D59">
+        <v>0.04</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>540</v>
+      </c>
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60">
+        <v>0.176</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0.002</v>
+      </c>
+      <c r="F60">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>541</v>
+      </c>
+      <c r="B61" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61">
+        <v>0.176</v>
+      </c>
+      <c r="D61">
+        <v>0.048</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <v>542</v>
+      </c>
+      <c r="B62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62">
+        <v>0.17</v>
+      </c>
+      <c r="D62">
+        <v>0.026</v>
+      </c>
+      <c r="E62">
+        <v>0.002</v>
+      </c>
+      <c r="F62">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <v>543</v>
+      </c>
+      <c r="B63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63">
+        <v>0.168</v>
+      </c>
+      <c r="D63">
+        <v>0.006</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <v>544</v>
+      </c>
+      <c r="B64" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64">
+        <v>0.214</v>
+      </c>
+      <c r="D64">
+        <v>0.058</v>
+      </c>
+      <c r="E64">
+        <v>0.002</v>
+      </c>
+      <c r="F64">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
+        <v>545</v>
+      </c>
+      <c r="B65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65">
+        <v>0.19</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66">
+        <v>546</v>
+      </c>
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66">
+        <v>0.202</v>
+      </c>
+      <c r="D66">
+        <v>0.014</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67">
+        <v>547</v>
+      </c>
+      <c r="B67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67">
+        <v>0.19</v>
+      </c>
+      <c r="D67">
+        <v>0.048</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68">
+        <v>548</v>
+      </c>
+      <c r="B68" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68">
+        <v>0.17</v>
+      </c>
+      <c r="D68">
+        <v>0.012</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69">
+        <v>549</v>
+      </c>
+      <c r="B69" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69">
+        <v>0.194</v>
+      </c>
+      <c r="D69">
+        <v>0.038</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70">
+        <v>550</v>
+      </c>
+      <c r="B70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70">
+        <v>0.208</v>
+      </c>
+      <c r="D70">
+        <v>0.058</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71">
+        <v>551</v>
+      </c>
+      <c r="B71" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71">
+        <v>0.394</v>
+      </c>
+      <c r="D71">
+        <v>0.022</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72">
+        <v>552</v>
+      </c>
+      <c r="B72" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72">
+        <v>0.48</v>
+      </c>
+      <c r="D72">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73">
+        <v>553</v>
+      </c>
+      <c r="B73" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73">
+        <v>0.342</v>
+      </c>
+      <c r="D73">
+        <v>0.024</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74">
+        <v>554</v>
+      </c>
+      <c r="B74" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74">
+        <v>0.232</v>
+      </c>
+      <c r="D74">
+        <v>0.006</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0.042</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75">
+        <v>555</v>
+      </c>
+      <c r="B75" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75">
+        <v>0.262</v>
+      </c>
+      <c r="D75">
+        <v>0.03</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0.044</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76">
+        <v>556</v>
+      </c>
+      <c r="B76" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76">
+        <v>0.244</v>
+      </c>
+      <c r="D76">
+        <v>0.026</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0.044</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77">
+        <v>557</v>
+      </c>
+      <c r="B77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77">
+        <v>0.212</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0.052</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78">
+        <v>558</v>
+      </c>
+      <c r="B78" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78">
+        <v>0.26</v>
+      </c>
+      <c r="D78">
+        <v>0.048</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79">
+        <v>559</v>
+      </c>
+      <c r="B79" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79">
+        <v>0.238</v>
+      </c>
+      <c r="D79">
+        <v>0.014</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80">
+        <v>560</v>
+      </c>
+      <c r="B80" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80">
+        <v>0.224</v>
+      </c>
+      <c r="D80">
+        <v>0.004</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0.046</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81">
+        <v>561</v>
+      </c>
+      <c r="B81" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81">
+        <v>0.258</v>
+      </c>
+      <c r="D81">
+        <v>0.056</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82">
+        <v>562</v>
+      </c>
+      <c r="B82" t="s">
+        <v>86</v>
+      </c>
+      <c r="C82">
+        <v>0.192</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0.052</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83">
+        <v>563</v>
+      </c>
+      <c r="B83" t="s">
+        <v>87</v>
+      </c>
+      <c r="C83">
+        <v>0.19</v>
+      </c>
+      <c r="D83">
+        <v>0.02</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84">
+        <v>564</v>
+      </c>
+      <c r="B84" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84">
+        <v>0.222</v>
+      </c>
+      <c r="D84">
+        <v>0.052</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85">
+        <v>565</v>
+      </c>
+      <c r="B85" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85">
+        <v>0.192</v>
+      </c>
+      <c r="D85">
+        <v>0.004</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86">
+        <v>566</v>
+      </c>
+      <c r="B86" t="s">
+        <v>90</v>
+      </c>
+      <c r="C86">
+        <v>0.192</v>
+      </c>
+      <c r="D86">
+        <v>0.034</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87">
+        <v>567</v>
+      </c>
+      <c r="B87" t="s">
+        <v>91</v>
+      </c>
+      <c r="C87">
+        <v>0.188</v>
+      </c>
+      <c r="D87">
+        <v>0.024</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88">
+        <v>568</v>
+      </c>
+      <c r="B88" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88">
+        <v>0.164</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89">
+        <v>569</v>
+      </c>
+      <c r="B89" t="s">
+        <v>93</v>
+      </c>
+      <c r="C89">
+        <v>0.198</v>
+      </c>
+      <c r="D89">
+        <v>0.058</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90">
+        <v>570</v>
+      </c>
+      <c r="B90" t="s">
+        <v>94</v>
+      </c>
+      <c r="C90">
+        <v>0.186</v>
+      </c>
+      <c r="D90">
+        <v>0.02</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91">
+        <v>571</v>
+      </c>
+      <c r="B91" t="s">
+        <v>95</v>
+      </c>
+      <c r="C91">
+        <v>0.298</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92">
+        <v>572</v>
+      </c>
+      <c r="B92" t="s">
+        <v>96</v>
+      </c>
+      <c r="C92">
+        <v>0.212</v>
+      </c>
+      <c r="D92">
+        <v>0.062</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93">
+        <v>573</v>
+      </c>
+      <c r="B93" t="s">
+        <v>97</v>
+      </c>
+      <c r="C93">
+        <v>0.15</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94">
+        <v>574</v>
+      </c>
+      <c r="B94" t="s">
+        <v>98</v>
+      </c>
+      <c r="C94">
+        <v>0.136</v>
+      </c>
+      <c r="D94">
+        <v>0.002</v>
+      </c>
+      <c r="E94">
+        <v>0.002</v>
+      </c>
+      <c r="F94">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95">
+        <v>575</v>
+      </c>
+      <c r="B95" t="s">
+        <v>99</v>
+      </c>
+      <c r="C95">
+        <v>0.16</v>
+      </c>
+      <c r="D95">
+        <v>0.082</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96">
+        <v>576</v>
+      </c>
+      <c r="B96" t="s">
+        <v>100</v>
+      </c>
+      <c r="C96">
+        <v>0.116</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0.002</v>
+      </c>
+      <c r="F96">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97">
+        <v>577</v>
+      </c>
+      <c r="B97" t="s">
+        <v>101</v>
+      </c>
+      <c r="C97">
+        <v>0.094</v>
+      </c>
+      <c r="D97">
+        <v>0.016</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98">
+        <v>578</v>
+      </c>
+      <c r="B98" t="s">
+        <v>197</v>
+      </c>
+      <c r="C98">
+        <v>0.15</v>
+      </c>
+      <c r="D98">
+        <v>0.05</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99">
+        <v>579</v>
+      </c>
+      <c r="B99" t="s">
+        <v>102</v>
+      </c>
+      <c r="C99">
+        <v>0.146</v>
+      </c>
+      <c r="D99">
+        <v>0.026</v>
+      </c>
+      <c r="E99">
+        <v>0.002</v>
+      </c>
+      <c r="F99">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100">
+        <v>580</v>
+      </c>
+      <c r="B100" t="s">
+        <v>103</v>
+      </c>
+      <c r="C100">
+        <v>0.122</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101">
+        <v>581</v>
+      </c>
+      <c r="B101" t="s">
+        <v>104</v>
+      </c>
+      <c r="C101">
+        <v>0.182</v>
+      </c>
+      <c r="D101">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E101">
+        <v>0.002</v>
+      </c>
+      <c r="F101">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102">
+        <v>582</v>
+      </c>
+      <c r="B102" t="s">
+        <v>105</v>
+      </c>
+      <c r="C102">
+        <v>0.174</v>
+      </c>
+      <c r="D102">
+        <v>0.018</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103">
+        <v>583</v>
+      </c>
+      <c r="B103" t="s">
+        <v>106</v>
+      </c>
+      <c r="C103">
+        <v>0.158</v>
+      </c>
+      <c r="D103">
+        <v>0.028</v>
+      </c>
+      <c r="E103">
+        <v>0.002</v>
+      </c>
+      <c r="F103">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104">
+        <v>584</v>
+      </c>
+      <c r="B104" t="s">
+        <v>107</v>
+      </c>
+      <c r="C104">
+        <v>0.212</v>
+      </c>
+      <c r="D104">
+        <v>0.04</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105">
+        <v>585</v>
+      </c>
+      <c r="B105" t="s">
+        <v>108</v>
+      </c>
+      <c r="C105">
+        <v>0.176</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0.002</v>
+      </c>
+      <c r="F105">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106">
+        <v>586</v>
+      </c>
+      <c r="B106" t="s">
+        <v>109</v>
+      </c>
+      <c r="C106">
+        <v>0.176</v>
+      </c>
+      <c r="D106">
+        <v>0.048</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107">
+        <v>587</v>
+      </c>
+      <c r="B107" t="s">
+        <v>110</v>
+      </c>
+      <c r="C107">
+        <v>0.17</v>
+      </c>
+      <c r="D107">
+        <v>0.026</v>
+      </c>
+      <c r="E107">
+        <v>0.002</v>
+      </c>
+      <c r="F107">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108">
+        <v>588</v>
+      </c>
+      <c r="B108" t="s">
+        <v>111</v>
+      </c>
+      <c r="C108">
+        <v>0.168</v>
+      </c>
+      <c r="D108">
+        <v>0.006</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109">
+        <v>589</v>
+      </c>
+      <c r="B109" t="s">
+        <v>112</v>
+      </c>
+      <c r="C109">
+        <v>0.214</v>
+      </c>
+      <c r="D109">
+        <v>0.058</v>
+      </c>
+      <c r="E109">
+        <v>0.002</v>
+      </c>
+      <c r="F109">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110">
+        <v>590</v>
+      </c>
+      <c r="B110" t="s">
+        <v>113</v>
+      </c>
+      <c r="C110">
+        <v>0.19</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111">
+        <v>591</v>
+      </c>
+      <c r="B111" t="s">
+        <v>114</v>
+      </c>
+      <c r="C111">
+        <v>0.202</v>
+      </c>
+      <c r="D111">
+        <v>0.014</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112">
+        <v>592</v>
+      </c>
+      <c r="B112" t="s">
+        <v>115</v>
+      </c>
+      <c r="C112">
+        <v>0.19</v>
+      </c>
+      <c r="D112">
+        <v>0.048</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113">
+        <v>593</v>
+      </c>
+      <c r="B113" t="s">
+        <v>116</v>
+      </c>
+      <c r="C113">
+        <v>0.17</v>
+      </c>
+      <c r="D113">
+        <v>0.012</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114">
+        <v>594</v>
+      </c>
+      <c r="B114" t="s">
+        <v>117</v>
+      </c>
+      <c r="C114">
+        <v>0.194</v>
+      </c>
+      <c r="D114">
+        <v>0.038</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115">
+        <v>595</v>
+      </c>
+      <c r="B115" t="s">
+        <v>118</v>
+      </c>
+      <c r="C115">
+        <v>0.208</v>
+      </c>
+      <c r="D115">
+        <v>0.058</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116">
+        <v>596</v>
+      </c>
+      <c r="B116" t="s">
+        <v>119</v>
+      </c>
+      <c r="C116">
+        <v>0.394</v>
+      </c>
+      <c r="D116">
+        <v>0.022</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117">
+        <v>597</v>
+      </c>
+      <c r="B117" t="s">
+        <v>120</v>
+      </c>
+      <c r="C117">
+        <v>0.48</v>
+      </c>
+      <c r="D117">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118">
+        <v>598</v>
+      </c>
+      <c r="B118" t="s">
+        <v>121</v>
+      </c>
+      <c r="C118">
+        <v>0.342</v>
+      </c>
+      <c r="D118">
+        <v>0.024</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119">
+        <v>599</v>
+      </c>
+      <c r="B119" t="s">
+        <v>122</v>
+      </c>
+      <c r="C119">
+        <v>0.232</v>
+      </c>
+      <c r="D119">
+        <v>0.006</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>0.042</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120">
+        <v>600</v>
+      </c>
+      <c r="B120" t="s">
+        <v>123</v>
+      </c>
+      <c r="C120">
+        <v>0.262</v>
+      </c>
+      <c r="D120">
+        <v>0.03</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>0.044</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121">
+        <v>601</v>
+      </c>
+      <c r="B121" t="s">
+        <v>124</v>
+      </c>
+      <c r="C121">
+        <v>0.244</v>
+      </c>
+      <c r="D121">
+        <v>0.026</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>0.044</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122">
+        <v>602</v>
+      </c>
+      <c r="B122" t="s">
+        <v>125</v>
+      </c>
+      <c r="C122">
+        <v>0.212</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>0.052</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123">
+        <v>603</v>
+      </c>
+      <c r="B123" t="s">
+        <v>126</v>
+      </c>
+      <c r="C123">
+        <v>0.26</v>
+      </c>
+      <c r="D123">
+        <v>0.048</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124">
+        <v>604</v>
+      </c>
+      <c r="B124" t="s">
+        <v>127</v>
+      </c>
+      <c r="C124">
+        <v>0.238</v>
+      </c>
+      <c r="D124">
+        <v>0.014</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125">
+        <v>605</v>
+      </c>
+      <c r="B125" t="s">
+        <v>128</v>
+      </c>
+      <c r="C125">
+        <v>0.224</v>
+      </c>
+      <c r="D125">
+        <v>0.004</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <v>0.046</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126">
+        <v>606</v>
+      </c>
+      <c r="B126" t="s">
+        <v>129</v>
+      </c>
+      <c r="C126">
+        <v>0.258</v>
+      </c>
+      <c r="D126">
+        <v>0.056</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127">
+        <v>607</v>
+      </c>
+      <c r="B127" t="s">
+        <v>130</v>
+      </c>
+      <c r="C127">
+        <v>0.192</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127">
+        <v>0.052</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128">
+        <v>608</v>
+      </c>
+      <c r="B128" t="s">
+        <v>131</v>
+      </c>
+      <c r="C128">
+        <v>0.19</v>
+      </c>
+      <c r="D128">
+        <v>0.02</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129">
+        <v>609</v>
+      </c>
+      <c r="B129" t="s">
+        <v>132</v>
+      </c>
+      <c r="C129">
+        <v>0.222</v>
+      </c>
+      <c r="D129">
+        <v>0.052</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130">
+        <v>610</v>
+      </c>
+      <c r="B130" t="s">
+        <v>133</v>
+      </c>
+      <c r="C130">
+        <v>0.192</v>
+      </c>
+      <c r="D130">
+        <v>0.004</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131">
+        <v>611</v>
+      </c>
+      <c r="B131" t="s">
+        <v>134</v>
+      </c>
+      <c r="C131">
+        <v>0.192</v>
+      </c>
+      <c r="D131">
+        <v>0.034</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132">
+        <v>612</v>
+      </c>
+      <c r="B132" t="s">
+        <v>135</v>
+      </c>
+      <c r="C132">
+        <v>0.188</v>
+      </c>
+      <c r="D132">
+        <v>0.024</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133">
+        <v>613</v>
+      </c>
+      <c r="B133" t="s">
+        <v>136</v>
+      </c>
+      <c r="C133">
+        <v>0.164</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134">
+        <v>614</v>
+      </c>
+      <c r="B134" t="s">
+        <v>137</v>
+      </c>
+      <c r="C134">
+        <v>0.198</v>
+      </c>
+      <c r="D134">
+        <v>0.058</v>
+      </c>
+      <c r="E134">
+        <v>0</v>
+      </c>
+      <c r="F134">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135">
+        <v>615</v>
+      </c>
+      <c r="B135" t="s">
+        <v>138</v>
+      </c>
+      <c r="C135">
+        <v>0.186</v>
+      </c>
+      <c r="D135">
+        <v>0.02</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136">
+        <v>616</v>
+      </c>
+      <c r="B136" t="s">
+        <v>139</v>
+      </c>
+      <c r="C136">
+        <v>0.298</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="F136">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137">
+        <v>617</v>
+      </c>
+      <c r="B137" t="s">
+        <v>140</v>
+      </c>
+      <c r="C137">
+        <v>0.212</v>
+      </c>
+      <c r="D137">
+        <v>0.062</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138">
+        <v>618</v>
+      </c>
+      <c r="B138" t="s">
+        <v>141</v>
+      </c>
+      <c r="C138">
+        <v>0.15</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139">
+        <v>619</v>
+      </c>
+      <c r="B139" t="s">
+        <v>142</v>
+      </c>
+      <c r="C139">
+        <v>0.136</v>
+      </c>
+      <c r="D139">
+        <v>0.002</v>
+      </c>
+      <c r="E139">
+        <v>0.002</v>
+      </c>
+      <c r="F139">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140">
+        <v>620</v>
+      </c>
+      <c r="B140" t="s">
+        <v>143</v>
+      </c>
+      <c r="C140">
+        <v>0.16</v>
+      </c>
+      <c r="D140">
+        <v>0.082</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141">
+        <v>621</v>
+      </c>
+      <c r="B141" t="s">
+        <v>144</v>
+      </c>
+      <c r="C141">
+        <v>0.116</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>0.002</v>
+      </c>
+      <c r="F141">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142">
+        <v>622</v>
+      </c>
+      <c r="B142" t="s">
+        <v>145</v>
+      </c>
+      <c r="C142">
+        <v>0.094</v>
+      </c>
+      <c r="D142">
+        <v>0.016</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <v>0.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F97"/>

</xml_diff>